<commit_message>
added BOM, deleted old gerbers
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="187">
   <si>
     <t>Qty</t>
   </si>
@@ -74,6 +74,18 @@
     <t>865080345012</t>
   </si>
   <si>
+    <t>C30, C31</t>
+  </si>
+  <si>
+    <t>6.8pF</t>
+  </si>
+  <si>
+    <t>399-C0402C689C5GAC7867CT-ND</t>
+  </si>
+  <si>
+    <t>C0402C689C5GAC7867</t>
+  </si>
+  <si>
     <t>C32</t>
   </si>
   <si>
@@ -212,10 +224,10 @@
     <t>Conn_01x04</t>
   </si>
   <si>
-    <t>WM4202-ND</t>
-  </si>
-  <si>
-    <t>0022232041</t>
+    <t>WM4330-ND</t>
+  </si>
+  <si>
+    <t>0470531000</t>
   </si>
   <si>
     <t>J5</t>
@@ -236,10 +248,16 @@
     <t>Conn_01x02</t>
   </si>
   <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>Conn_02x06_Odd_Even</t>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-F-DV-K</t>
+  </si>
+  <si>
+    <t>SAM8796-ND</t>
   </si>
   <si>
     <t>JP1, JP2</t>
@@ -254,6 +272,12 @@
     <t>SolderJumper_2_Bridged</t>
   </si>
   <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>JTAG Source</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -284,16 +308,7 @@
     <t>YAG2306CT-ND</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>311-33.0LRCT-ND</t>
-  </si>
-  <si>
-    <t>R3, R5, R23</t>
+    <t>R2, R3, R5, R23</t>
   </si>
   <si>
     <t>0</t>
@@ -302,7 +317,7 @@
     <t>RMCF0402ZT0R00CT-ND</t>
   </si>
   <si>
-    <t>R4, R6, R9, R20, R24, R30, R31, R32, R33, R34, R35, R36</t>
+    <t>R4, R6, R9, R20, R24, R36</t>
   </si>
   <si>
     <t>10k</t>
@@ -416,7 +431,7 @@
     <t>YAG3078CT-ND</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP19, TP20, TP21, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32</t>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32</t>
   </si>
   <si>
     <t>TestPoint</t>
@@ -549,6 +564,18 @@
   </si>
   <si>
     <t>ESP32-S3-WROOM-1-N16R8</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
+  </si>
+  <si>
+    <t>728-1074-1-ND</t>
+  </si>
+  <si>
+    <t>SC32S-7PF20PPM</t>
   </si>
 </sst>
 </file>
@@ -908,7 +935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1000,7 +1027,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -1011,36 +1038,39 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1048,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1062,13 +1092,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1076,41 +1106,41 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1118,16 +1148,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1135,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1149,7 +1176,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -1157,16 +1184,16 @@
       <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>53</v>
@@ -1174,44 +1201,44 @@
       <c r="C17" t="s">
         <v>54</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
         <v>56</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
         <v>60</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
@@ -1219,8 +1246,11 @@
       <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" t="s">
-        <v>52</v>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1228,16 +1258,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
         <v>66</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1250,8 +1277,11 @@
       <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="F22" t="s">
-        <v>52</v>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1259,13 +1289,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1273,13 +1303,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1287,27 +1317,27 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1315,35 +1345,32 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" t="s">
-        <v>52</v>
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" t="s">
         <v>82</v>
+      </c>
+      <c r="F28" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
@@ -1351,25 +1378,19 @@
       <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="D29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
+      <c r="F29" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
         <v>86</v>
-      </c>
-      <c r="C30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1377,83 +1398,92 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>90</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>93</v>
       </c>
-      <c r="D32" t="s">
-        <v>94</v>
+      <c r="E32" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
         <v>95</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>96</v>
       </c>
-      <c r="D33" t="s">
-        <v>97</v>
+      <c r="F33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>99</v>
-      </c>
-      <c r="D34" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>102</v>
-      </c>
-      <c r="D35" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>105</v>
-      </c>
-      <c r="D36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1461,13 +1491,13 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
         <v>107</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>108</v>
-      </c>
-      <c r="D37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1475,13 +1505,13 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
         <v>110</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>111</v>
-      </c>
-      <c r="D38" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1489,13 +1519,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
         <v>113</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>114</v>
-      </c>
-      <c r="D39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1503,13 +1533,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" t="s">
         <v>116</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>117</v>
-      </c>
-      <c r="D40" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1517,13 +1547,13 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
         <v>119</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>120</v>
-      </c>
-      <c r="D41" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1531,27 +1561,27 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
         <v>122</v>
       </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" t="s">
-        <v>52</v>
+      <c r="D42" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1559,13 +1589,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" t="s">
-        <v>128</v>
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1573,46 +1603,46 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" t="s">
         <v>129</v>
       </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" t="s">
-        <v>52</v>
+        <v>104</v>
+      </c>
+      <c r="D47" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
         <v>135</v>
@@ -1623,200 +1653,245 @@
       <c r="D48" t="s">
         <v>137</v>
       </c>
-      <c r="E48" t="s">
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>31</v>
+      </c>
+      <c r="B49" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>139</v>
       </c>
-      <c r="C49" t="s">
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
         <v>140</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C50" t="s">
         <v>141</v>
       </c>
-      <c r="E49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>142</v>
-      </c>
-      <c r="C50" t="s">
-        <v>143</v>
-      </c>
-      <c r="D50" t="s">
-        <v>144</v>
       </c>
       <c r="E50" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6">
       <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>2</v>
       </c>
-      <c r="B51" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" t="s">
-        <v>146</v>
-      </c>
-      <c r="D51" t="s">
-        <v>147</v>
-      </c>
-      <c r="E51" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B53" t="s">
         <v>150</v>
       </c>
-      <c r="D52" t="s">
+      <c r="C53" t="s">
         <v>151</v>
       </c>
-      <c r="E52" t="s">
+      <c r="D53" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="E53" t="s">
         <v>153</v>
       </c>
-      <c r="C53" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" t="s">
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>154</v>
       </c>
-      <c r="E53" t="s">
+      <c r="C54" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>156</v>
       </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>157</v>
       </c>
-      <c r="D54" t="s">
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
         <v>158</v>
       </c>
-      <c r="E54" t="s">
+      <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="E55" t="s">
         <v>160</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
         <v>161</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C56" t="s">
         <v>162</v>
       </c>
-      <c r="E55" t="s">
+      <c r="D56" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="E56" t="s">
         <v>164</v>
       </c>
-      <c r="C56" t="s">
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
+      <c r="C57" t="s">
         <v>166</v>
       </c>
-      <c r="E56" t="s">
+      <c r="D57" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="E57" t="s">
         <v>168</v>
       </c>
-      <c r="C57" t="s">
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
         <v>169</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C58" t="s">
         <v>170</v>
       </c>
-      <c r="E57" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>171</v>
-      </c>
-      <c r="C58" t="s">
-        <v>172</v>
-      </c>
-      <c r="D58" t="s">
-        <v>173</v>
       </c>
       <c r="E58" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>1</v>
       </c>
       <c r="B59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" t="s">
         <v>174</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>175</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
         <v>176</v>
       </c>
-      <c r="E59" t="s">
+      <c r="C60" t="s">
         <v>177</v>
+      </c>
+      <c r="D60" t="s">
+        <v>178</v>
+      </c>
+      <c r="E60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>183</v>
+      </c>
+      <c r="C62" t="s">
+        <v>184</v>
+      </c>
+      <c r="D62" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E16" r:id="rId1"/>
+    <hyperlink ref="E17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1824,7 +1899,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1891,7 +1966,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -1902,24 +1977,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1927,10 +2002,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1938,10 +2013,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1949,32 +2024,32 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1982,10 +2057,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1993,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
@@ -2001,24 +2076,24 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2026,32 +2101,29 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2059,54 +2131,54 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
         <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2114,10 +2186,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2125,10 +2197,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2136,10 +2208,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2147,10 +2219,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2158,10 +2230,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2169,43 +2241,43 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2213,15 +2285,15 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
         <v>135</v>
@@ -2235,10 +2307,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2246,32 +2318,32 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2279,10 +2351,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2290,10 +2362,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2301,10 +2373,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2312,10 +2384,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2323,10 +2395,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2334,10 +2406,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2345,10 +2417,32 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
-        <v>176</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added manufacturing files. clarified MCP1824 part names
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxeMax/Manufacturing Files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAF303D-6AEE-BD48-A82D-919953EE021C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="34640" windowHeight="24540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="DK Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="188">
   <si>
     <t>Qty</t>
   </si>
@@ -576,13 +582,16 @@
   </si>
   <si>
     <t>SC32S-7PF20PPM</t>
+  </si>
+  <si>
+    <t>C2-6, C8, C10-12, C14-18, C24, C25, C27, C35, C44, C49, C50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +656,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -693,7 +710,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -725,9 +742,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -759,6 +794,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -934,19 +987,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +1019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>13</v>
       </c>
@@ -980,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>21</v>
       </c>
@@ -994,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1008,7 +1061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1025,7 +1078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1042,7 +1095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1056,7 +1109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1073,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1087,7 +1140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1101,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1115,7 +1168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1129,7 +1182,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1143,7 +1196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1157,7 +1210,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1174,7 +1227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1191,7 +1244,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1208,7 +1261,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1222,7 +1275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1236,7 +1289,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1253,7 +1306,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1267,7 +1320,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1284,7 +1337,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1298,7 +1351,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1312,7 +1365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1326,7 +1379,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1340,7 +1393,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1354,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1368,7 +1421,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1382,7 +1435,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1392,8 +1445,11 @@
       <c r="C30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1410,7 +1466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1427,7 +1483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1444,7 +1500,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1458,7 +1514,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6</v>
       </c>
@@ -1472,7 +1528,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1486,7 +1542,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1500,7 +1556,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1514,7 +1570,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1528,7 +1584,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1542,7 +1598,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1556,7 +1612,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1570,7 +1626,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1584,7 +1640,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1598,7 +1654,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1612,7 +1668,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1626,7 +1682,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1640,7 +1696,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1654,7 +1710,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>31</v>
       </c>
@@ -1668,7 +1724,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1685,7 +1741,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -1702,7 +1758,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1719,7 +1775,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1736,7 +1792,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1753,7 +1809,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -1770,7 +1826,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1787,7 +1843,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1804,7 +1860,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1821,7 +1877,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1838,7 +1894,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1855,7 +1911,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -1872,7 +1928,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1891,25 +1947,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1"/>
+    <hyperlink ref="E17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="4" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1931,18 +1991,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1953,7 +2013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1964,7 +2024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1975,7 +2035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1986,7 +2046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1997,7 +2057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2008,7 +2068,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2019,7 +2079,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2030,7 +2090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2041,7 +2101,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2052,7 +2112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2063,7 +2123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2074,7 +2134,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2085,7 +2145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2096,7 +2156,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2107,7 +2167,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2118,330 +2178,322 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>6</v>
-      </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>131</v>
-      </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39">
-        <v>1</v>
-      </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>183</v>
-      </c>
-      <c r="C49" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added manufacturer part numbers to schematic and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxeMax/Manufacturing Files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAF303D-6AEE-BD48-A82D-919953EE021C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="34640" windowHeight="24540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="DK Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="211">
   <si>
     <t>Qty</t>
   </si>
@@ -50,6 +44,9 @@
     <t>1292-1639-1-ND</t>
   </si>
   <si>
+    <t>0402X104K100CT</t>
+  </si>
+  <si>
     <t>C2, C3, C4, C5, C6, C8, C10, C11, C12, C14, C15, C16, C17, C18, C24, C25, C27, C35, C44, C49, C50</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
     <t>587-5514-1-ND</t>
   </si>
   <si>
+    <t>EMK105BJ105MV-F</t>
+  </si>
+  <si>
     <t>C13</t>
   </si>
   <si>
@@ -68,6 +68,9 @@
     <t>718-1028-1-ND</t>
   </si>
   <si>
+    <t>293D337X9010E2TE3</t>
+  </si>
+  <si>
     <t>C28</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
     <t>1276-1566-1-ND</t>
   </si>
   <si>
+    <t>CL05B471KB5NNNC</t>
+  </si>
+  <si>
     <t>C34, C36, C37</t>
   </si>
   <si>
@@ -119,6 +125,9 @@
     <t>1276-6471-1-ND</t>
   </si>
   <si>
+    <t>CL21B105KOFNNNG</t>
+  </si>
+  <si>
     <t>C39</t>
   </si>
   <si>
@@ -128,6 +137,9 @@
     <t>1276-1552-1-ND</t>
   </si>
   <si>
+    <t>CL05B332KB5NNNC</t>
+  </si>
+  <si>
     <t>C40</t>
   </si>
   <si>
@@ -137,6 +149,9 @@
     <t>311-1114-1-ND</t>
   </si>
   <si>
+    <t>CC0805JRNPO9BN181</t>
+  </si>
+  <si>
     <t>C41</t>
   </si>
   <si>
@@ -146,6 +161,9 @@
     <t>311-1128-1-ND</t>
   </si>
   <si>
+    <t>CC0805KRX7R9BB152</t>
+  </si>
+  <si>
     <t>C43, C51</t>
   </si>
   <si>
@@ -155,12 +173,18 @@
     <t>1276-1096-1-ND</t>
   </si>
   <si>
+    <t>CL21A106KOQNNNE</t>
+  </si>
+  <si>
     <t>C45</t>
   </si>
   <si>
     <t>1292-1580-1-ND</t>
   </si>
   <si>
+    <t>0805B471K500CT</t>
+  </si>
+  <si>
     <t>C46</t>
   </si>
   <si>
@@ -323,6 +347,9 @@
     <t>RMCF0402ZT0R00CT-ND</t>
   </si>
   <si>
+    <t>RMCF0402ZT0R00</t>
+  </si>
+  <si>
     <t>R4, R6, R9, R20, R24, R36</t>
   </si>
   <si>
@@ -332,6 +359,9 @@
     <t>311-10KJRCT-ND</t>
   </si>
   <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
     <t>R7, R8</t>
   </si>
   <si>
@@ -341,6 +371,9 @@
     <t>RMCF0402FT100RCT-ND</t>
   </si>
   <si>
+    <t>RMCF0402FT100R</t>
+  </si>
+  <si>
     <t>R10</t>
   </si>
   <si>
@@ -350,6 +383,9 @@
     <t>311-3.83KLRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-073K83L</t>
+  </si>
+  <si>
     <t>R11</t>
   </si>
   <si>
@@ -359,6 +395,9 @@
     <t>311-100KJRCT-ND</t>
   </si>
   <si>
+    <t>RC0402JR-07100KL</t>
+  </si>
+  <si>
     <t>R12</t>
   </si>
   <si>
@@ -368,6 +407,9 @@
     <t>RMCF0402FT4K12CT-ND</t>
   </si>
   <si>
+    <t>RMCF0402FT4K12</t>
+  </si>
+  <si>
     <t>R13</t>
   </si>
   <si>
@@ -377,6 +419,9 @@
     <t>311-1.33KLRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-071K33L</t>
+  </si>
+  <si>
     <t>R14</t>
   </si>
   <si>
@@ -386,6 +431,9 @@
     <t>311-4.99KLRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-074K99L</t>
+  </si>
+  <si>
     <t>R15</t>
   </si>
   <si>
@@ -395,6 +443,9 @@
     <t>311-3.32KLRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-073K32L</t>
+  </si>
+  <si>
     <t>R16</t>
   </si>
   <si>
@@ -404,6 +455,9 @@
     <t>311-80.6KLRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-0780K6L</t>
+  </si>
+  <si>
     <t>R17</t>
   </si>
   <si>
@@ -416,6 +470,9 @@
     <t>311-60.4LRCT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-0760R4L</t>
+  </si>
+  <si>
     <t>R25</t>
   </si>
   <si>
@@ -425,6 +482,9 @@
     <t>YAG3027CT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-0719R1L</t>
+  </si>
+  <si>
     <t>R26, R27</t>
   </si>
   <si>
@@ -437,6 +497,9 @@
     <t>YAG3078CT-ND</t>
   </si>
   <si>
+    <t>RC0402FR-07261RL</t>
+  </si>
+  <si>
     <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32</t>
   </si>
   <si>
@@ -488,7 +551,7 @@
     <t>U5</t>
   </si>
   <si>
-    <t>MCP1824</t>
+    <t>MCP1824T-1802E</t>
   </si>
   <si>
     <t>MCP1824T-1802E/OTCT-ND</t>
@@ -500,6 +563,9 @@
     <t>U6</t>
   </si>
   <si>
+    <t>MCP1824T-0802E</t>
+  </si>
+  <si>
     <t>MCP1824T-0802E/OTCT-ND</t>
   </si>
   <si>
@@ -582,16 +648,13 @@
   </si>
   <si>
     <t>SC32S-7PF20PPM</t>
-  </si>
-  <si>
-    <t>C2-6, C8, C10-12, C14-18, C24, C25, C27, C35, C44, C49, C50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,14 +719,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -710,7 +765,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,27 +797,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -794,24 +831,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -987,19 +1006,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1032,944 +1051,1015 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
         <v>66</v>
       </c>
-      <c r="F21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="E37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="E39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="E40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="E42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="E47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="D50" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="E50" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="E53" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="E55" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="D56" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="E56" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="D57" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="E57" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="D58" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="E58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C59" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="D59" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="E59" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D60" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="D61" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="E61" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C62" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="D62" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="E62" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C48"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="57.6640625" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +2070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1991,510 +2081,510 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="C39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="C47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed R1 from schematic and ROM to address #42 and prolly #35
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="210">
   <si>
     <t>Qty</t>
   </si>
@@ -329,136 +329,133 @@
     <t>296-27625-1-ND</t>
   </si>
   <si>
-    <t>R1, R18, R19</t>
+    <t>R2, R3, R5, R23</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00</t>
+  </si>
+  <si>
+    <t>R4, R6, R9, R20, R24, R36</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>311-10KJRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>RMCF0402FT100RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT100R</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>3.83k</t>
+  </si>
+  <si>
+    <t>311-3.83KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-073K83L</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>311-100KJRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-07100KL</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>4.12k</t>
+  </si>
+  <si>
+    <t>RMCF0402FT4K12CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT4K12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>1.33k</t>
+  </si>
+  <si>
+    <t>311-1.33KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-071K33L</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>311-4.99KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-074K99L</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>3.32k</t>
+  </si>
+  <si>
+    <t>311-3.32KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-073K32L</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>80k</t>
+  </si>
+  <si>
+    <t>311-80.6KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-0780K6L</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18, R19</t>
   </si>
   <si>
     <t>1k</t>
-  </si>
-  <si>
-    <t>YAG2306CT-ND</t>
-  </si>
-  <si>
-    <t>R2, R3, R5, R23</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>RMCF0402ZT0R00CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402ZT0R00</t>
-  </si>
-  <si>
-    <t>R4, R6, R9, R20, R24, R36</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>311-10KJRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402JR-0710KL</t>
-  </si>
-  <si>
-    <t>R7, R8</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>RMCF0402FT100RCT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402FT100R</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>3.83k</t>
-  </si>
-  <si>
-    <t>311-3.83KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-073K83L</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>311-100KJRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402JR-07100KL</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>4.12k</t>
-  </si>
-  <si>
-    <t>RMCF0402FT4K12CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402FT4K12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>1.33k</t>
-  </si>
-  <si>
-    <t>311-1.33KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-071K33L</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>4.99k</t>
-  </si>
-  <si>
-    <t>311-4.99KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-074K99L</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>3.32k</t>
-  </si>
-  <si>
-    <t>311-3.32KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-073K32L</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>80k</t>
-  </si>
-  <si>
-    <t>311-80.6KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-0780K6L</t>
-  </si>
-  <si>
-    <t>R17</t>
   </si>
   <si>
     <t>R21, R22</t>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>104</v>
@@ -1548,59 +1545,59 @@
       <c r="D33" t="s">
         <v>106</v>
       </c>
-      <c r="F33" t="s">
-        <v>66</v>
+      <c r="E33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1608,16 +1605,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1625,16 +1622,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1642,16 +1639,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1659,16 +1656,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1676,16 +1673,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1693,16 +1690,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1710,27 +1707,24 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" t="s">
-        <v>145</v>
-      </c>
-      <c r="E43" t="s">
-        <v>146</v>
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F44" t="s">
         <v>66</v>
@@ -1741,16 +1735,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" t="s">
         <v>148</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>149</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>150</v>
-      </c>
-      <c r="E45" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1758,16 +1752,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" t="s">
         <v>152</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>153</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>154</v>
-      </c>
-      <c r="E46" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1775,16 +1769,16 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1792,16 +1786,16 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" t="s">
         <v>157</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>158</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>159</v>
-      </c>
-      <c r="E48" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1809,10 +1803,10 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" t="s">
         <v>161</v>
-      </c>
-      <c r="C49" t="s">
-        <v>162</v>
       </c>
       <c r="F49" t="s">
         <v>66</v>
@@ -1823,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>164</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>165</v>
-      </c>
-      <c r="E50" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1840,16 +1834,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" t="s">
         <v>167</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>168</v>
       </c>
-      <c r="D51" t="s">
-        <v>169</v>
-      </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1857,16 +1851,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" t="s">
         <v>170</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>171</v>
       </c>
-      <c r="D52" t="s">
-        <v>172</v>
-      </c>
       <c r="E52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1874,16 +1868,16 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" t="s">
         <v>173</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>174</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>175</v>
-      </c>
-      <c r="E53" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1891,16 +1885,16 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
         <v>177</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>178</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>179</v>
-      </c>
-      <c r="E54" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1908,16 +1902,16 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" t="s">
         <v>181</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>182</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>183</v>
-      </c>
-      <c r="E55" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1925,16 +1919,16 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" t="s">
         <v>185</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>186</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>187</v>
-      </c>
-      <c r="E56" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1942,16 +1936,16 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
         <v>189</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>190</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>191</v>
-      </c>
-      <c r="E57" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1959,16 +1953,16 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" t="s">
         <v>193</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>194</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>195</v>
-      </c>
-      <c r="E58" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1976,16 +1970,16 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" t="s">
         <v>197</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>198</v>
       </c>
-      <c r="D59" t="s">
-        <v>199</v>
-      </c>
       <c r="E59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1993,16 +1987,16 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" t="s">
         <v>200</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>201</v>
       </c>
-      <c r="D60" t="s">
-        <v>202</v>
-      </c>
       <c r="E60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2010,16 +2004,16 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" t="s">
         <v>203</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>204</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>205</v>
-      </c>
-      <c r="E61" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2027,16 +2021,16 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" t="s">
         <v>207</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>208</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>209</v>
-      </c>
-      <c r="E62" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2295,10 +2289,10 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2306,10 +2300,10 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2317,10 +2311,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2328,10 +2322,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2339,10 +2333,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2350,10 +2344,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2361,10 +2355,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2372,10 +2366,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2383,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2394,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2405,10 +2399,10 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2416,10 +2410,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2427,10 +2421,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2438,10 +2432,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2449,10 +2443,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2460,10 +2454,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2471,10 +2465,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2482,10 +2476,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2493,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2504,10 +2498,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2515,10 +2509,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2526,10 +2520,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2537,10 +2531,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2548,10 +2542,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2559,10 +2553,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2570,10 +2564,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2581,10 +2575,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some v2.2 DNP parts
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="210">
   <si>
     <t>Qty</t>
   </si>
@@ -47,6 +47,9 @@
     <t>0402X104K100CT</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>C2, C3, C4, C5, C6, C8, C10, C11, C12, C14, C15, C16, C17, C18, C24, C25, C27, C35, C44, C49, C50</t>
   </si>
   <si>
@@ -213,9 +216,6 @@
   </si>
   <si>
     <t>https://www.amazon.com/dp/B07MDFS1YS</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>H5, H6</t>
@@ -1051,22 +1051,25 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1074,16 +1077,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1091,16 +1094,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1108,16 +1111,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1125,16 +1128,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1142,16 +1145,16 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1159,16 +1162,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1176,16 +1179,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1193,16 +1196,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1210,16 +1213,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1227,16 +1230,16 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1244,16 +1247,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1261,16 +1264,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1278,16 +1281,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1295,16 +1298,16 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1318,7 +1321,7 @@
         <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1332,7 +1335,7 @@
         <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1363,7 +1366,7 @@
         <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1394,7 +1397,7 @@
         <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1408,7 +1411,7 @@
         <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1422,7 +1425,7 @@
         <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1436,7 +1439,7 @@
         <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1467,7 +1470,7 @@
         <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1481,7 +1484,7 @@
         <v>94</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1495,7 +1498,7 @@
         <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1548,6 +1551,9 @@
       <c r="E33" t="s">
         <v>107</v>
       </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
@@ -1565,6 +1571,9 @@
       <c r="E34" t="s">
         <v>111</v>
       </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
@@ -1713,7 +1722,7 @@
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1727,7 +1736,7 @@
         <v>146</v>
       </c>
       <c r="F44" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1763,6 +1772,9 @@
       <c r="E46" t="s">
         <v>154</v>
       </c>
+      <c r="F46" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
@@ -1809,7 +1821,7 @@
         <v>161</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1861,6 +1873,9 @@
       </c>
       <c r="E52" t="s">
         <v>170</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2043,7 +2058,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2066,24 +2081,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2091,54 +2106,54 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2146,10 +2161,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2157,10 +2172,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2168,32 +2183,32 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2201,10 +2216,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2212,32 +2227,32 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2245,10 +2260,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2256,21 +2271,21 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2278,43 +2293,43 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2322,10 +2337,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2333,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2344,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2355,54 +2370,54 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2410,10 +2425,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2421,21 +2436,21 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2443,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2454,10 +2469,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2465,21 +2480,21 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="C38" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2487,10 +2502,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="C40" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2498,10 +2513,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C41" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2509,10 +2524,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C42" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2520,64 +2535,9 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="C43" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>202</v>
-      </c>
-      <c r="C47" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>206</v>
-      </c>
-      <c r="C48" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the DNP BOM issues
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeMax BOM.xlsx
+++ b/Manufacturing Files/bitaxeMax BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="194">
   <si>
     <t>Qty</t>
   </si>
@@ -35,7 +35,7 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>C1, C7, C9, C19, C20, C21, C22, C23, C26, C29, C33, C42, C52</t>
+    <t>C1, C7, C9, C19, C20, C22, C23, C29, C33, C42, C52</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -47,9 +47,6 @@
     <t>0402X104K100CT</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>C2, C3, C4, C5, C6, C8, C10, C11, C12, C14, C15, C16, C17, C18, C24, C25, C27, C35, C44, C49, C50</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
     <t>293D337X9010E2TE3</t>
   </si>
   <si>
+    <t>C21, C26</t>
+  </si>
+  <si>
     <t>C28</t>
   </si>
   <si>
@@ -209,21 +209,6 @@
     <t>C3216X5R0J107M160AB</t>
   </si>
   <si>
-    <t>H1, H2, H3, H4</t>
-  </si>
-  <si>
-    <t>AlignmentHole</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B07MDFS1YS</t>
-  </si>
-  <si>
-    <t>H5, H6</t>
-  </si>
-  <si>
-    <t>MountingHole</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -260,27 +245,12 @@
     <t>0470531000</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>TC2030-IDC</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>Conn_01x08</t>
-  </si>
-  <si>
     <t>J7</t>
   </si>
   <si>
     <t>Conn_01x02</t>
   </si>
   <si>
-    <t>J9</t>
-  </si>
-  <si>
     <t>J10</t>
   </si>
   <si>
@@ -290,24 +260,6 @@
     <t>SAM8796-ND</t>
   </si>
   <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Open</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Bridged</t>
-  </si>
-  <si>
-    <t>JP4</t>
-  </si>
-  <si>
-    <t>JTAG Source</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -329,7 +281,7 @@
     <t>296-27625-1-ND</t>
   </si>
   <si>
-    <t>R2, R3, R5, R23</t>
+    <t>R2, R3, R5</t>
   </si>
   <si>
     <t>0</t>
@@ -341,7 +293,7 @@
     <t>RMCF0402ZT0R00</t>
   </si>
   <si>
-    <t>R4, R6, R9, R20, R24, R36</t>
+    <t>R4, R6, R9, R20, R36</t>
   </si>
   <si>
     <t>10k</t>
@@ -470,6 +422,12 @@
     <t>RC0402FR-0760R4L</t>
   </si>
   <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
     <t>R25</t>
   </si>
   <si>
@@ -495,12 +453,6 @@
   </si>
   <si>
     <t>RC0402FR-07261RL</t>
-  </si>
-  <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
   </si>
   <si>
     <t>U1</t>
@@ -651,7 +603,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,13 +618,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -698,20 +643,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1004,7 +943,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1037,7 +976,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1050,9 +989,6 @@
       </c>
       <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1060,16 +996,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1077,101 +1013,104 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1179,16 +1118,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1196,16 +1135,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1213,50 +1152,50 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1264,16 +1203,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1281,142 +1220,139 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>85</v>
@@ -1424,172 +1360,181 @@
       <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="F25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F33" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1597,50 +1542,44 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>119</v>
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" t="s">
-        <v>123</v>
+        <v>130</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1648,16 +1587,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>91</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1665,16 +1607,19 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1682,78 +1627,87 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="E42" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" t="s">
         <v>144</v>
       </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" t="s">
-        <v>10</v>
+      <c r="E43" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1761,19 +1715,19 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E46" t="s">
         <v>154</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1781,284 +1735,179 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="E47" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E48" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
-      </c>
-      <c r="F49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D50" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E50" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D51" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E51" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D52" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E52" t="s">
-        <v>170</v>
-      </c>
-      <c r="F52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C53" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D53" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E53" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E54" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C55" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D55" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E55" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C56" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D56" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E56" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
-        <v>188</v>
-      </c>
-      <c r="C57" t="s">
-        <v>189</v>
-      </c>
-      <c r="D57" t="s">
-        <v>190</v>
-      </c>
-      <c r="E57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
-        <v>192</v>
-      </c>
-      <c r="C58" t="s">
         <v>193</v>
       </c>
-      <c r="D58" t="s">
-        <v>194</v>
-      </c>
-      <c r="E58" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>196</v>
-      </c>
-      <c r="C59" t="s">
-        <v>197</v>
-      </c>
-      <c r="D59" t="s">
-        <v>198</v>
-      </c>
-      <c r="E59" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
-        <v>199</v>
-      </c>
-      <c r="C60" t="s">
-        <v>200</v>
-      </c>
-      <c r="D60" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
-        <v>202</v>
-      </c>
-      <c r="C61" t="s">
-        <v>203</v>
-      </c>
-      <c r="D61" t="s">
-        <v>204</v>
-      </c>
-      <c r="E61" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
-        <v>206</v>
-      </c>
-      <c r="C62" t="s">
-        <v>207</v>
-      </c>
-      <c r="D62" t="s">
-        <v>208</v>
-      </c>
-      <c r="E62" t="s">
-        <v>209</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2081,24 +1930,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2106,54 +1955,54 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2161,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2172,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2183,32 +2032,32 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2216,10 +2065,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2227,21 +2076,21 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2249,21 +2098,18 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2271,32 +2117,26 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2304,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2315,54 +2155,54 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2370,43 +2210,43 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2414,10 +2254,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2425,54 +2265,54 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2480,10 +2320,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2491,21 +2331,21 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2513,10 +2353,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2524,10 +2364,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2535,10 +2375,76 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>